<commit_message>
Removed low n species
update to script 1 to remove species with too few specimens (so far)
</commit_message>
<xml_diff>
--- a/Data/Results/18_12_17_static_allometry_pairwise_comp.xlsx
+++ b/Data/Results/18_12_17_static_allometry_pairwise_comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aemarcy/Documents/Work/Science/Research/2018 3 Crania Morph/aus-rodent-skulls/Data/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47475F9E-69C7-D54B-BCDB-ED562B840FAA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9774FC0C-51D1-184E-A51C-919DED491FF6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="27240" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -972,11 +972,15 @@
   <dimension ref="A1:AJ36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z1" sqref="Z1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
+    <col min="34" max="34" width="7.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B1" t="s">

</xml_diff>